<commit_message>
Started creating the equations of motion of the 14 dof vehicle model from the SAE paper, and integrating it in the laptime simulation algorithm
However, the simulation times are increadible high, and there are many challenges related to find the ideal initial guess
</commit_message>
<xml_diff>
--- a/+Model/LMP2_Bas.xlsx
+++ b/+Model/LMP2_Bas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\LaptimeSimOCP\+Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B0ED8FC-CBB9-44F7-86C5-E3995F6EB006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41FFB2ED-4827-4AA9-945D-C1098D56FEF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8880" firstSheet="2" activeTab="7" xr2:uid="{C9770ACA-89D6-4C25-A406-8CFD34B6BEB6}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8880" activeTab="5" xr2:uid="{C9770ACA-89D6-4C25-A406-8CFD34B6BEB6}"/>
   </bookViews>
   <sheets>
     <sheet name="MassInertia" sheetId="1" r:id="rId1"/>
@@ -537,7 +537,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -606,7 +606,7 @@
         <v>4.4939999999999998</v>
       </c>
       <c r="I2">
-        <v>0.316</v>
+        <v>0.43</v>
       </c>
       <c r="J2">
         <f>0.47</f>
@@ -871,8 +871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2744984F-2619-4555-ADE9-32DB97027A3A}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -912,7 +912,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -951,7 +951,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E935BBC8-6905-40C4-93AA-35113AE6796F}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>